<commit_message>
small fixes + tornado diagram
</commit_message>
<xml_diff>
--- a/data-raw/8c_cost_utilisation_diagnostics.xlsx
+++ b/data-raw/8c_cost_utilisation_diagnostics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67302623-AD06-AD45-B791-239F6D811195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430F5A8F-ED29-5A43-82DF-8365B61F815B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37060" yWindow="1100" windowWidth="33600" windowHeight="20500" xr2:uid="{9DDAF4C6-8B12-DE46-894E-28C14AE1ACDC}"/>
   </bookViews>
@@ -252,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +271,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
     </font>
   </fonts>
   <fills count="4">
@@ -320,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -331,6 +336,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D11125-B8EC-AE49-AA97-1F0EF4C235C9}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -658,6 +664,7 @@
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1">
@@ -680,7 +687,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1">
+    <row r="2" spans="1:6" ht="19" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -696,11 +703,11 @@
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1">
+      <c r="F2" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -716,8 +723,8 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>120.05</v>
+      <c r="F3" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" thickBot="1">
@@ -736,8 +743,8 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4">
-        <v>120.05</v>
+      <c r="F4" s="4">
+        <v>53.006666666666597</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" thickBot="1">
@@ -756,8 +763,8 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>120.05</v>
+      <c r="F5" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" thickBot="1">
@@ -776,11 +783,11 @@
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" thickBot="1">
+      <c r="F6" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -796,11 +803,11 @@
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7">
-        <v>61.92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1">
+      <c r="F7" s="4">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -816,8 +823,8 @@
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F8">
-        <v>148.02000000000001</v>
+      <c r="F8" s="4">
+        <v>60.3</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43" thickBot="1">
@@ -836,11 +843,11 @@
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F9">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1">
+      <c r="F9" s="4">
+        <v>40.016666666666602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -856,11 +863,11 @@
       <c r="E10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F10">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" thickBot="1">
+      <c r="F10" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -876,8 +883,8 @@
       <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F11">
-        <v>120.05</v>
+      <c r="F11" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" thickBot="1">
@@ -896,8 +903,8 @@
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>120.05</v>
+      <c r="F12" s="4">
+        <v>53.006666666666597</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" thickBot="1">
@@ -916,8 +923,8 @@
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13">
-        <v>120.05</v>
+      <c r="F13" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29" thickBot="1">
@@ -936,11 +943,11 @@
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" thickBot="1">
+      <c r="F14" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="19" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -956,11 +963,11 @@
       <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F15">
-        <v>61.92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" thickBot="1">
+      <c r="F15" s="4">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="19" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -976,8 +983,8 @@
       <c r="E16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F16">
-        <v>148.02000000000001</v>
+      <c r="F16" s="4">
+        <v>60.3</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43" thickBot="1">
@@ -996,11 +1003,11 @@
       <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F17">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1">
+      <c r="F17" s="4">
+        <v>40.016666666666602</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1016,11 +1023,11 @@
       <c r="E18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F18">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" thickBot="1">
+      <c r="F18" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1036,8 +1043,8 @@
       <c r="E19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F19">
-        <v>120.05</v>
+      <c r="F19" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" thickBot="1">
@@ -1056,8 +1063,8 @@
       <c r="E20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F20">
-        <v>120.05</v>
+      <c r="F20" s="4">
+        <v>53.006666666666597</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" thickBot="1">
@@ -1076,8 +1083,8 @@
       <c r="E21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F21">
-        <v>120.05</v>
+      <c r="F21" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="29" thickBot="1">
@@ -1096,11 +1103,11 @@
       <c r="E22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" thickBot="1">
+      <c r="F22" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="19" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
@@ -1116,11 +1123,11 @@
       <c r="E23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F23">
-        <v>61.92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" thickBot="1">
+      <c r="F23" s="4">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="19" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1136,8 +1143,8 @@
       <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F24">
-        <v>148.02000000000001</v>
+      <c r="F24" s="4">
+        <v>60.3</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43" thickBot="1">
@@ -1156,11 +1163,11 @@
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F25">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" thickBot="1">
+      <c r="F25" s="4">
+        <v>40.016666666666602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="19" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1176,11 +1183,11 @@
       <c r="E26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F26">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" thickBot="1">
+      <c r="F26" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="19" thickBot="1">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -1196,8 +1203,8 @@
       <c r="E27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F27">
-        <v>120.05</v>
+      <c r="F27" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" thickBot="1">
@@ -1216,8 +1223,8 @@
       <c r="E28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F28">
-        <v>120.05</v>
+      <c r="F28" s="4">
+        <v>53.006666666666597</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="29" thickBot="1">
@@ -1236,8 +1243,8 @@
       <c r="E29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F29">
-        <v>120.05</v>
+      <c r="F29" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" thickBot="1">
@@ -1256,11 +1263,11 @@
       <c r="E30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" thickBot="1">
+      <c r="F30" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="19" thickBot="1">
       <c r="A31" s="2" t="s">
         <v>50</v>
       </c>
@@ -1276,11 +1283,11 @@
       <c r="E31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F31">
-        <v>61.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" thickBot="1">
+      <c r="F31" s="4">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="19" thickBot="1">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
@@ -1296,8 +1303,8 @@
       <c r="E32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F32">
-        <v>148.02000000000001</v>
+      <c r="F32" s="4">
+        <v>60.3</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43" thickBot="1">
@@ -1316,11 +1323,11 @@
       <c r="E33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F33">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="17" thickBot="1">
+      <c r="F33" s="4">
+        <v>40.016666666666602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="19" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -1336,11 +1343,11 @@
       <c r="E34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F34">
-        <v>120.05</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="17" thickBot="1">
+      <c r="F34" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="19" thickBot="1">
       <c r="A35" s="2" t="s">
         <v>55</v>
       </c>
@@ -1356,8 +1363,8 @@
       <c r="E35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F35">
-        <v>120.05</v>
+      <c r="F35" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" thickBot="1">
@@ -1376,8 +1383,8 @@
       <c r="E36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F36">
-        <v>120.05</v>
+      <c r="F36" s="4">
+        <v>53.006666666666597</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="29" thickBot="1">
@@ -1396,8 +1403,8 @@
       <c r="E37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F37">
-        <v>120.05</v>
+      <c r="F37" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" thickBot="1">
@@ -1416,11 +1423,11 @@
       <c r="E38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="17" thickBot="1">
+      <c r="F38" s="4">
+        <v>53.006666666666597</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="19" thickBot="1">
       <c r="A39" s="2" t="s">
         <v>59</v>
       </c>
@@ -1436,11 +1443,11 @@
       <c r="E39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F39">
-        <v>61.92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="17" thickBot="1">
+      <c r="F39" s="4">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="19" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -1456,8 +1463,8 @@
       <c r="E40" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F40">
-        <v>148.02000000000001</v>
+      <c r="F40" s="4">
+        <v>60.3</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="43" thickBot="1">
@@ -1476,8 +1483,8 @@
       <c r="E41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F41">
-        <v>120.05</v>
+      <c r="F41" s="4">
+        <v>40.016666666666602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement dsa / tornadoplot
</commit_message>
<xml_diff>
--- a/data-raw/8c_cost_utilisation_diagnostics.xlsx
+++ b/data-raw/8c_cost_utilisation_diagnostics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430F5A8F-ED29-5A43-82DF-8365B61F815B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3726031-7F89-594B-A4CC-CBD6E59FD669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37060" yWindow="1100" windowWidth="33600" windowHeight="20500" xr2:uid="{9DDAF4C6-8B12-DE46-894E-28C14AE1ACDC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{9DDAF4C6-8B12-DE46-894E-28C14AE1ACDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -355,9 +355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -395,7 +395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -501,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D11125-B8EC-AE49-AA97-1F0EF4C235C9}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -704,10 +704,10 @@
         <v>2</v>
       </c>
       <c r="F2" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -723,7 +723,7 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -743,8 +743,8 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="4">
-        <v>53.006666666666597</v>
+      <c r="F4">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" thickBot="1">
@@ -763,8 +763,8 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
-        <v>40.016666666666602</v>
+      <c r="F5">
+        <v>39.020000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" thickBot="1">
@@ -783,11 +783,11 @@
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19" thickBot="1">
+      <c r="F6">
+        <v>79.510000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -803,8 +803,8 @@
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="4">
-        <v>60.3</v>
+      <c r="F7">
+        <v>40.47</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19" thickBot="1">
@@ -824,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="4">
-        <v>60.3</v>
+        <v>171.71</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43" thickBot="1">
@@ -843,7 +843,7 @@
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -864,10 +864,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="19" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="E11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -903,8 +903,8 @@
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="4">
-        <v>53.006666666666597</v>
+      <c r="F12">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" thickBot="1">
@@ -923,8 +923,8 @@
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="4">
-        <v>40.016666666666602</v>
+      <c r="F13">
+        <v>39.020000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29" thickBot="1">
@@ -943,11 +943,11 @@
       <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="19" thickBot="1">
+      <c r="F14">
+        <v>79.510000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -963,8 +963,8 @@
       <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="4">
-        <v>60.3</v>
+      <c r="F15">
+        <v>40.47</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19" thickBot="1">
@@ -984,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="4">
-        <v>60.3</v>
+        <v>171.71</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43" thickBot="1">
@@ -1003,7 +1003,7 @@
       <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -1024,10 +1024,10 @@
         <v>2</v>
       </c>
       <c r="F18" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="19" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1043,7 +1043,7 @@
       <c r="E19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -1063,8 +1063,8 @@
       <c r="E20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="4">
-        <v>53.006666666666597</v>
+      <c r="F20">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" thickBot="1">
@@ -1083,8 +1083,8 @@
       <c r="E21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="4">
-        <v>40.016666666666602</v>
+      <c r="F21">
+        <v>39.020000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="29" thickBot="1">
@@ -1103,11 +1103,11 @@
       <c r="E22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="19" thickBot="1">
+      <c r="F22">
+        <v>79.510000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
@@ -1123,8 +1123,8 @@
       <c r="E23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="4">
-        <v>60.3</v>
+      <c r="F23">
+        <v>40.47</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="19" thickBot="1">
@@ -1144,7 +1144,7 @@
         <v>36</v>
       </c>
       <c r="F24" s="4">
-        <v>60.3</v>
+        <v>171.71</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43" thickBot="1">
@@ -1163,7 +1163,7 @@
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -1184,10 +1184,10 @@
         <v>2</v>
       </c>
       <c r="F26" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="19" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" thickBot="1">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="E27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -1223,8 +1223,8 @@
       <c r="E28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="4">
-        <v>53.006666666666597</v>
+      <c r="F28">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="29" thickBot="1">
@@ -1243,8 +1243,8 @@
       <c r="E29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="4">
-        <v>40.016666666666602</v>
+      <c r="F29">
+        <v>39.020000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" thickBot="1">
@@ -1263,11 +1263,11 @@
       <c r="E30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="19" thickBot="1">
+      <c r="F30">
+        <v>79.510000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" thickBot="1">
       <c r="A31" s="2" t="s">
         <v>50</v>
       </c>
@@ -1283,8 +1283,8 @@
       <c r="E31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="4">
-        <v>60.3</v>
+      <c r="F31">
+        <v>40.47</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="19" thickBot="1">
@@ -1304,7 +1304,7 @@
         <v>36</v>
       </c>
       <c r="F32" s="4">
-        <v>60.3</v>
+        <v>171.71</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43" thickBot="1">
@@ -1323,7 +1323,7 @@
       <c r="E33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -1344,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="F34" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="19" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" thickBot="1">
       <c r="A35" s="2" t="s">
         <v>55</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="E35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35">
         <v>40.016666666666602</v>
       </c>
     </row>
@@ -1383,8 +1383,8 @@
       <c r="E36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="4">
-        <v>53.006666666666597</v>
+      <c r="F36">
+        <v>40.016666666666602</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="29" thickBot="1">
@@ -1403,8 +1403,8 @@
       <c r="E37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="4">
-        <v>40.016666666666602</v>
+      <c r="F37">
+        <v>39.020000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" thickBot="1">
@@ -1423,11 +1423,11 @@
       <c r="E38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F38" s="4">
-        <v>53.006666666666597</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="19" thickBot="1">
+      <c r="F38">
+        <v>79.510000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" thickBot="1">
       <c r="A39" s="2" t="s">
         <v>59</v>
       </c>
@@ -1443,8 +1443,8 @@
       <c r="E39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="4">
-        <v>60.3</v>
+      <c r="F39">
+        <v>40.47</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="19" thickBot="1">
@@ -1464,7 +1464,7 @@
         <v>54</v>
       </c>
       <c r="F40" s="4">
-        <v>60.3</v>
+        <v>171.71</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="43" thickBot="1">
@@ -1483,7 +1483,7 @@
       <c r="E41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41">
         <v>40.016666666666602</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some bugg fixesx + transition probs
</commit_message>
<xml_diff>
--- a/data-raw/8c_cost_utilisation_diagnostics.xlsx
+++ b/data-raw/8c_cost_utilisation_diagnostics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3726031-7F89-594B-A4CC-CBD6E59FD669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59891AAC-6B57-624F-AE5C-02EB0530762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{9DDAF4C6-8B12-DE46-894E-28C14AE1ACDC}"/>
   </bookViews>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>0.35</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>diagnosis_1_obs</t>
   </si>
   <si>
@@ -65,18 +59,12 @@
     <t xml:space="preserve">    Angle assessment (kamerhoek)</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>diagnosis_4_obs</t>
   </si>
   <si>
     <t xml:space="preserve">    Intraocular pressure assessment</t>
   </si>
   <si>
-    <t>0.4</t>
-  </si>
-  <si>
     <t>diangosis_5_obs</t>
   </si>
   <si>
@@ -95,9 +83,6 @@
     <t xml:space="preserve">    Visual field test</t>
   </si>
   <si>
-    <t>0.1</t>
-  </si>
-  <si>
     <t>diagnosis_8_obs</t>
   </si>
   <si>
@@ -137,33 +122,18 @@
     <t>diagnosis_1_mod</t>
   </si>
   <si>
-    <t>0.3</t>
-  </si>
-  <si>
     <t>diagnosis_2_mod</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
     <t>diagnosis_3_mod</t>
   </si>
   <si>
     <t>diagnosis_4_mod</t>
   </si>
   <si>
-    <t>6.0</t>
-  </si>
-  <si>
     <t>diangosis_5_mod</t>
   </si>
   <si>
-    <t>0.25</t>
-  </si>
-  <si>
     <t>diagnosis_6_mod</t>
   </si>
   <si>
@@ -200,9 +170,6 @@
     <t>diagnosis_1_blind</t>
   </si>
   <si>
-    <t>0.05</t>
-  </si>
-  <si>
     <t>diagnosis_2_blind</t>
   </si>
   <si>
@@ -218,25 +185,13 @@
     <t>diagnosis_6_blind</t>
   </si>
   <si>
-    <t>0.01</t>
-  </si>
-  <si>
     <t>diagnosis_7_blind</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
     <t>diagnosis_8_blind</t>
   </si>
   <si>
     <t>average_best</t>
-  </si>
-  <si>
-    <t>average_lowest</t>
-  </si>
-  <si>
-    <t>average_highest</t>
   </si>
   <si>
     <t>name</t>
@@ -653,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D11125-B8EC-AE49-AA97-1F0EF4C235C9}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -669,823 +624,629 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="19" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
+      <c r="C2" s="2">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="D2" s="2">
+        <v>120.05</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>40.016666666666602</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.55999999999999994</v>
+      </c>
+      <c r="D3" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="29" thickBot="1">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>40.016666666666602</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="D4" s="2">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="29" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="D5" s="1">
         <v>39.020000000000003</v>
       </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="29" thickBot="1">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="D6" s="2">
         <v>79.510000000000005</v>
       </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="17" thickBot="1">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="D7" s="1">
         <v>40.47</v>
       </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="19" thickBot="1">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="D8" s="2">
         <v>171.71</v>
       </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="43" thickBot="1">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>40.016666666666602</v>
-      </c>
+      <c r="D9" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="19" thickBot="1">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
+      <c r="C10" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>120.05</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="17" thickBot="1">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>40.016666666666602</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="29" thickBot="1">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>40.016666666666602</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="D12" s="2">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="29" thickBot="1">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="D13" s="1">
         <v>39.020000000000003</v>
       </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="29" thickBot="1">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="D14" s="2">
         <v>79.510000000000005</v>
       </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="17" thickBot="1">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="D15" s="1">
         <v>40.47</v>
       </c>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="19" thickBot="1">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="4">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="D16" s="2">
         <v>171.71</v>
       </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="43" thickBot="1">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>40.016666666666602</v>
-      </c>
+      <c r="D17" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="19" thickBot="1">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
+      <c r="C18" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>120.05</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="17" thickBot="1">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19">
-        <v>40.016666666666602</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="29" thickBot="1">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>40.016666666666602</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="2">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="29" thickBot="1">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D21" s="1">
         <v>39.020000000000003</v>
       </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="29" thickBot="1">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="D22" s="2">
         <v>79.510000000000005</v>
       </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="17" thickBot="1">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.1199999999999999</v>
+      </c>
+      <c r="D23" s="1">
         <v>40.47</v>
       </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="19" thickBot="1">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="4">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="D24" s="2">
         <v>171.71</v>
       </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="43" thickBot="1">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25">
-        <v>40.016666666666602</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D25" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="19" thickBot="1">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="4">
-        <v>0</v>
-      </c>
+      <c r="C26" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>120.05</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="17" thickBot="1">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27">
-        <v>40.016666666666602</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="29" thickBot="1">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
         <v>1</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28">
-        <v>40.016666666666602</v>
-      </c>
+      <c r="D28" s="2">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="29" thickBot="1">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D29" s="1">
         <v>39.020000000000003</v>
       </c>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="29" thickBot="1">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="D30" s="2">
         <v>79.510000000000005</v>
       </c>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="17" thickBot="1">
       <c r="A31" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F31">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="D31" s="1">
         <v>40.47</v>
       </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="19" thickBot="1">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="4">
+        <v>14</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="D32" s="2">
         <v>171.71</v>
       </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="43" thickBot="1">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33">
-        <v>40.016666666666602</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D33" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="19" thickBot="1">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>120.05</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="17" thickBot="1">
       <c r="A35" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35">
-        <v>40.016666666666602</v>
-      </c>
+      <c r="D35" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="29" thickBot="1">
       <c r="A36" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36">
-        <v>40.016666666666602</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:6" ht="29" thickBot="1">
       <c r="A37" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D37" s="1">
         <v>39.020000000000003</v>
       </c>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="29" thickBot="1">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="D38" s="2">
         <v>79.510000000000005</v>
       </c>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6" ht="17" thickBot="1">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="D39" s="1">
         <v>40.47</v>
       </c>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="19" thickBot="1">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F40" s="4">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="D40" s="2">
         <v>171.71</v>
       </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="43" thickBot="1">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41">
-        <v>40.016666666666602</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D41" s="1">
+        <v>40.016666669999999</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished scenario + plot
</commit_message>
<xml_diff>
--- a/data-raw/8c_cost_utilisation_diagnostics.xlsx
+++ b/data-raw/8c_cost_utilisation_diagnostics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59891AAC-6B57-624F-AE5C-02EB0530762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5DE8EB-FEE3-AC45-BF26-4BB9FD32F229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{9DDAF4C6-8B12-DE46-894E-28C14AE1ACDC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="21100" xr2:uid="{9DDAF4C6-8B12-DE46-894E-28C14AE1ACDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>0.35</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>lower_bound</t>
+  </si>
+  <si>
+    <t>upper_bound</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D11125-B8EC-AE49-AA97-1F0EF4C235C9}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -617,12 +623,13 @@
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:8" ht="17" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -633,12 +640,18 @@
         <v>51</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="19" thickBot="1">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="19" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -649,12 +662,18 @@
         <v>0.52600000000000002</v>
       </c>
       <c r="D2" s="2">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F2" s="2">
         <v>120.05</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1">
+      <c r="G2" s="2"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -665,11 +684,17 @@
         <v>0.55999999999999994</v>
       </c>
       <c r="D3" s="1">
+        <v>0.28600000000000003</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.1199999999999999</v>
+      </c>
+      <c r="F3" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="29" thickBot="1">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="29" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -680,11 +705,17 @@
         <v>0.45999999999999996</v>
       </c>
       <c r="D4" s="2">
+        <v>0.20600000000000002</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="F4" s="2">
         <v>40.016666669999999</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="29" thickBot="1">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="29" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -695,11 +726,17 @@
         <v>0.52600000000000002</v>
       </c>
       <c r="D5" s="1">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F5" s="1">
         <v>39.020000000000003</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="29" thickBot="1">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -710,11 +747,17 @@
         <v>0.18</v>
       </c>
       <c r="D6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F6" s="2">
         <v>79.510000000000005</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" thickBot="1">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -725,11 +768,17 @@
         <v>0.52600000000000002</v>
       </c>
       <c r="D7" s="1">
+        <v>0.2666</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F7" s="1">
         <v>40.47</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="19" thickBot="1">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="19" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -740,12 +789,18 @@
         <v>0.22000000000000003</v>
       </c>
       <c r="D8" s="2">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F8" s="2">
         <v>171.71</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="43" thickBot="1">
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="43" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -756,11 +811,17 @@
         <v>0</v>
       </c>
       <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="19" thickBot="1">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="19" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -771,12 +832,18 @@
         <v>1.4</v>
       </c>
       <c r="D10" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="F10" s="2">
         <v>120.05</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="17" thickBot="1">
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -787,11 +854,17 @@
         <v>1.2</v>
       </c>
       <c r="D11" s="1">
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.12</v>
+      </c>
+      <c r="F11" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="29" thickBot="1">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -802,11 +875,17 @@
         <v>0.65</v>
       </c>
       <c r="D12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="F12" s="2">
         <v>40.016666669999999</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="29" thickBot="1">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="29" thickBot="1">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -817,11 +896,17 @@
         <v>1.4</v>
       </c>
       <c r="D13" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F13" s="1">
         <v>39.020000000000003</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="29" thickBot="1">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="29" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -832,11 +917,17 @@
         <v>0.34</v>
       </c>
       <c r="D14" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="F14" s="2">
         <v>79.510000000000005</v>
       </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="17" thickBot="1">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" thickBot="1">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -847,11 +938,17 @@
         <v>1.02</v>
       </c>
       <c r="D15" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
         <v>40.47</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="19" thickBot="1">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="19" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -862,12 +959,18 @@
         <v>0.95</v>
       </c>
       <c r="D16" s="2">
+        <v>0.48000000000000009</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="F16" s="2">
         <v>171.71</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" ht="43" thickBot="1">
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="43" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -878,11 +981,17 @@
         <v>0</v>
       </c>
       <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="19" thickBot="1">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="19" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -893,12 +1002,18 @@
         <v>1.6</v>
       </c>
       <c r="D18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="F18" s="2">
         <v>120.05</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="17" thickBot="1">
+      <c r="G18" s="2"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -909,11 +1024,17 @@
         <v>1.3</v>
       </c>
       <c r="D19" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2.52</v>
+      </c>
+      <c r="F19" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="29" thickBot="1">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="29" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -924,11 +1045,17 @@
         <v>0.7</v>
       </c>
       <c r="D20" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.3800000000000001</v>
+      </c>
+      <c r="F20" s="2">
         <v>40.016666669999999</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="29" thickBot="1">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="29" thickBot="1">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -939,11 +1066,17 @@
         <v>1.6</v>
       </c>
       <c r="D21" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="F21" s="1">
         <v>39.020000000000003</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="29" thickBot="1">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="29" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -954,11 +1087,17 @@
         <v>0.34</v>
       </c>
       <c r="D22" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="F22" s="2">
         <v>79.510000000000005</v>
       </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="17" thickBot="1">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -969,11 +1108,17 @@
         <v>1.1199999999999999</v>
       </c>
       <c r="D23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.02</v>
+      </c>
+      <c r="F23" s="1">
         <v>40.47</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="19" thickBot="1">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="19" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -984,12 +1129,18 @@
         <v>1.04</v>
       </c>
       <c r="D24" s="2">
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.16</v>
+      </c>
+      <c r="F24" s="2">
         <v>171.71</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" ht="43" thickBot="1">
+      <c r="G24" s="2"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="43" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1000,11 +1151,17 @@
         <v>25</v>
       </c>
       <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="19" thickBot="1">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="19" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1015,12 +1172,18 @@
         <v>2.5</v>
       </c>
       <c r="D26" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="F26" s="2">
         <v>120.05</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" ht="17" thickBot="1">
+      <c r="G26" s="2"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="17" thickBot="1">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1031,11 +1194,17 @@
         <v>2</v>
       </c>
       <c r="D27" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3.5200000000000005</v>
+      </c>
+      <c r="F27" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="29" thickBot="1">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="29" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -1046,11 +1215,17 @@
         <v>1</v>
       </c>
       <c r="D28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.6800000000000002</v>
+      </c>
+      <c r="F28" s="2">
         <v>40.016666669999999</v>
       </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="29" thickBot="1">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="29" thickBot="1">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1061,11 +1236,17 @@
         <v>2.5</v>
       </c>
       <c r="D29" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="F29" s="1">
         <v>39.020000000000003</v>
       </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="29" thickBot="1">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="29" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1076,11 +1257,17 @@
         <v>0.34</v>
       </c>
       <c r="D30" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="F30" s="2">
         <v>79.510000000000005</v>
       </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" ht="17" thickBot="1">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="17" thickBot="1">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
@@ -1091,11 +1278,17 @@
         <v>1.17</v>
       </c>
       <c r="D31" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2.57</v>
+      </c>
+      <c r="F31" s="1">
         <v>40.47</v>
       </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="19" thickBot="1">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="19" thickBot="1">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1106,12 +1299,18 @@
         <v>1.7</v>
       </c>
       <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="F32" s="2">
         <v>171.71</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="43" thickBot="1">
+      <c r="G32" s="2"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="43" thickBot="1">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1122,11 +1321,17 @@
         <v>25</v>
       </c>
       <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" ht="19" thickBot="1">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="19" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -1137,12 +1342,18 @@
         <v>2.5</v>
       </c>
       <c r="D34" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="F34" s="2">
         <v>120.05</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" ht="17" thickBot="1">
+      <c r="G34" s="2"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="17" thickBot="1">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -1153,11 +1364,17 @@
         <v>2</v>
       </c>
       <c r="D35" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3.5200000000000005</v>
+      </c>
+      <c r="F35" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="29" thickBot="1">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="29" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
@@ -1168,11 +1385,17 @@
         <v>1</v>
       </c>
       <c r="D36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.6800000000000002</v>
+      </c>
+      <c r="F36" s="2">
         <v>40.016666669999999</v>
       </c>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="29" thickBot="1">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="29" thickBot="1">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -1183,11 +1406,17 @@
         <v>2.5</v>
       </c>
       <c r="D37" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="E37" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="F37" s="1">
         <v>39.020000000000003</v>
       </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="29" thickBot="1">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="29" thickBot="1">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -1198,11 +1427,17 @@
         <v>0.34</v>
       </c>
       <c r="D38" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="F38" s="2">
         <v>79.510000000000005</v>
       </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="17" thickBot="1">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" ht="17" thickBot="1">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
@@ -1213,11 +1448,17 @@
         <v>1.17</v>
       </c>
       <c r="D39" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E39" s="1">
+        <v>2.57</v>
+      </c>
+      <c r="F39" s="1">
         <v>40.47</v>
       </c>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="19" thickBot="1">
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" ht="19" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
@@ -1228,12 +1469,18 @@
         <v>1.7</v>
       </c>
       <c r="D40" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E40" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="F40" s="2">
         <v>171.71</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" ht="43" thickBot="1">
+      <c r="G40" s="2"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="43" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
@@ -1244,9 +1491,15 @@
         <v>26</v>
       </c>
       <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
         <v>40.016666669999999</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>